<commit_message>
with all federal holidays added!
</commit_message>
<xml_diff>
--- a/2021_cboc_signin_sheets/02February_2021_cboc_signin_sheet.xlsx
+++ b/2021_cboc_signin_sheets/02February_2021_cboc_signin_sheet.xlsx
@@ -746,8 +746,8 @@
     <col customWidth="1" max="27" min="27" width="2.5"/>
     <col customWidth="1" max="28" min="28" width="2.5"/>
     <col customWidth="1" max="29" min="29" width="2.5"/>
-    <col customWidth="1" max="30" min="30" width="4.5"/>
-    <col customWidth="1" max="31" min="31" width="4.5"/>
+    <col customWidth="1" max="30" min="30" width="2.5"/>
+    <col customWidth="1" max="31" min="31" width="2.5"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="45" r="1">
@@ -877,12 +877,12 @@
         </is>
       </c>
       <c r="AC2" s="8" t="n"/>
-      <c r="AD2" s="5" t="inlineStr">
+      <c r="AD2" s="7" t="inlineStr">
         <is>
           <t>MON</t>
         </is>
       </c>
-      <c r="AE2" s="6" t="n"/>
+      <c r="AE2" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="22" r="3">
       <c r="A3" s="9" t="inlineStr">
@@ -946,10 +946,10 @@
         <v>14</v>
       </c>
       <c r="AC3" s="8" t="n"/>
-      <c r="AD3" s="5" t="n">
+      <c r="AD3" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="AE3" s="6" t="n"/>
+      <c r="AE3" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="27" r="4">
       <c r="A4" s="10" t="n"/>
@@ -1093,12 +1093,12 @@
           <t>Time of Arrival</t>
         </is>
       </c>
-      <c r="AD4" s="11" t="inlineStr">
+      <c r="AD4" s="13" t="inlineStr">
         <is>
           <t>Tech</t>
         </is>
       </c>
-      <c r="AE4" s="12" t="inlineStr">
+      <c r="AE4" s="14" t="inlineStr">
         <is>
           <t>Time of Arrival</t>
         </is>
@@ -1170,8 +1170,16 @@
           <t>X</t>
         </is>
       </c>
-      <c r="AD5" s="16" t="n"/>
-      <c r="AE5" s="17" t="n"/>
+      <c r="AD5" s="18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE5" s="19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="6">
       <c r="A6" s="20" t="inlineStr">
@@ -1239,8 +1247,16 @@
           <t>X</t>
         </is>
       </c>
-      <c r="AD6" s="21" t="n"/>
-      <c r="AE6" s="22" t="n"/>
+      <c r="AD6" s="23" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE6" s="24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="10" r="7">
       <c r="A7" s="10" t="n"/>
@@ -1272,8 +1288,8 @@
       <c r="AA7" s="28" t="n"/>
       <c r="AB7" s="27" t="n"/>
       <c r="AC7" s="28" t="n"/>
-      <c r="AD7" s="25" t="n"/>
-      <c r="AE7" s="26" t="n"/>
+      <c r="AD7" s="27" t="n"/>
+      <c r="AE7" s="28" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="8">
       <c r="A8" s="15" t="inlineStr">
@@ -1341,8 +1357,16 @@
           <t>X</t>
         </is>
       </c>
-      <c r="AD8" s="16" t="n"/>
-      <c r="AE8" s="17" t="n"/>
+      <c r="AD8" s="18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE8" s="19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="9">
       <c r="A9" s="20" t="inlineStr">
@@ -1410,8 +1434,16 @@
           <t>X</t>
         </is>
       </c>
-      <c r="AD9" s="21" t="n"/>
-      <c r="AE9" s="22" t="n"/>
+      <c r="AD9" s="23" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE9" s="24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="10" r="10">
       <c r="A10" s="10" t="n"/>
@@ -1443,8 +1475,8 @@
       <c r="AA10" s="28" t="n"/>
       <c r="AB10" s="27" t="n"/>
       <c r="AC10" s="28" t="n"/>
-      <c r="AD10" s="25" t="n"/>
-      <c r="AE10" s="26" t="n"/>
+      <c r="AD10" s="27" t="n"/>
+      <c r="AE10" s="28" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="11">
       <c r="A11" s="15" t="inlineStr">
@@ -1512,8 +1544,16 @@
           <t>X</t>
         </is>
       </c>
-      <c r="AD11" s="16" t="n"/>
-      <c r="AE11" s="17" t="n"/>
+      <c r="AD11" s="18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE11" s="19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="12">
       <c r="A12" s="20" t="inlineStr">
@@ -1581,8 +1621,16 @@
           <t>X</t>
         </is>
       </c>
-      <c r="AD12" s="21" t="n"/>
-      <c r="AE12" s="22" t="n"/>
+      <c r="AD12" s="23" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE12" s="24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="10" r="13">
       <c r="A13" s="10" t="n"/>
@@ -1614,8 +1662,8 @@
       <c r="AA13" s="28" t="n"/>
       <c r="AB13" s="27" t="n"/>
       <c r="AC13" s="28" t="n"/>
-      <c r="AD13" s="25" t="n"/>
-      <c r="AE13" s="26" t="n"/>
+      <c r="AD13" s="27" t="n"/>
+      <c r="AE13" s="28" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="14">
       <c r="A14" s="15" t="inlineStr">
@@ -1683,8 +1731,16 @@
           <t>X</t>
         </is>
       </c>
-      <c r="AD14" s="16" t="n"/>
-      <c r="AE14" s="17" t="n"/>
+      <c r="AD14" s="18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE14" s="19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="15">
       <c r="A15" s="20" t="inlineStr">
@@ -1752,8 +1808,16 @@
           <t>X</t>
         </is>
       </c>
-      <c r="AD15" s="21" t="n"/>
-      <c r="AE15" s="22" t="n"/>
+      <c r="AD15" s="23" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE15" s="24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="10" r="16">
       <c r="A16" s="10" t="n"/>
@@ -1785,8 +1849,8 @@
       <c r="AA16" s="28" t="n"/>
       <c r="AB16" s="27" t="n"/>
       <c r="AC16" s="28" t="n"/>
-      <c r="AD16" s="25" t="n"/>
-      <c r="AE16" s="26" t="n"/>
+      <c r="AD16" s="27" t="n"/>
+      <c r="AE16" s="28" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="17">
       <c r="A17" s="15" t="inlineStr">
@@ -1854,8 +1918,16 @@
           <t>X</t>
         </is>
       </c>
-      <c r="AD17" s="16" t="n"/>
-      <c r="AE17" s="17" t="n"/>
+      <c r="AD17" s="18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE17" s="19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="18">
       <c r="A18" s="20" t="inlineStr">
@@ -1923,8 +1995,16 @@
           <t>X</t>
         </is>
       </c>
-      <c r="AD18" s="21" t="n"/>
-      <c r="AE18" s="22" t="n"/>
+      <c r="AD18" s="23" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE18" s="24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="10" r="19">
       <c r="A19" s="10" t="n"/>
@@ -1956,8 +2036,8 @@
       <c r="AA19" s="28" t="n"/>
       <c r="AB19" s="27" t="n"/>
       <c r="AC19" s="28" t="n"/>
-      <c r="AD19" s="25" t="n"/>
-      <c r="AE19" s="26" t="n"/>
+      <c r="AD19" s="27" t="n"/>
+      <c r="AE19" s="28" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="20">
       <c r="A20" s="15" t="inlineStr">
@@ -2025,8 +2105,16 @@
           <t>X</t>
         </is>
       </c>
-      <c r="AD20" s="16" t="n"/>
-      <c r="AE20" s="17" t="n"/>
+      <c r="AD20" s="18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE20" s="19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="21">
       <c r="A21" s="20" t="inlineStr">
@@ -2094,8 +2182,16 @@
           <t>X</t>
         </is>
       </c>
-      <c r="AD21" s="21" t="n"/>
-      <c r="AE21" s="22" t="n"/>
+      <c r="AD21" s="23" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE21" s="24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="10" r="22">
       <c r="A22" s="10" t="n"/>
@@ -2127,8 +2223,8 @@
       <c r="AA22" s="28" t="n"/>
       <c r="AB22" s="27" t="n"/>
       <c r="AC22" s="28" t="n"/>
-      <c r="AD22" s="25" t="n"/>
-      <c r="AE22" s="26" t="n"/>
+      <c r="AD22" s="27" t="n"/>
+      <c r="AE22" s="28" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="23">
       <c r="A23" s="15" t="inlineStr">
@@ -2196,8 +2292,16 @@
           <t>X</t>
         </is>
       </c>
-      <c r="AD23" s="16" t="n"/>
-      <c r="AE23" s="17" t="n"/>
+      <c r="AD23" s="18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE23" s="19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="24">
       <c r="A24" s="20" t="inlineStr">
@@ -2265,8 +2369,16 @@
           <t>X</t>
         </is>
       </c>
-      <c r="AD24" s="21" t="n"/>
-      <c r="AE24" s="22" t="n"/>
+      <c r="AD24" s="23" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE24" s="24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="10" r="25">
       <c r="A25" s="10" t="n"/>
@@ -2298,8 +2410,8 @@
       <c r="AA25" s="28" t="n"/>
       <c r="AB25" s="27" t="n"/>
       <c r="AC25" s="28" t="n"/>
-      <c r="AD25" s="25" t="n"/>
-      <c r="AE25" s="26" t="n"/>
+      <c r="AD25" s="27" t="n"/>
+      <c r="AE25" s="28" t="n"/>
     </row>
     <row customHeight="1" ht="21" r="26">
       <c r="A26" s="15" t="inlineStr">
@@ -2367,8 +2479,16 @@
           <t>X</t>
         </is>
       </c>
-      <c r="AD26" s="16" t="n"/>
-      <c r="AE26" s="17" t="n"/>
+      <c r="AD26" s="18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE26" s="19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="21" r="27">
       <c r="A27" s="9" t="inlineStr">
@@ -2436,8 +2556,16 @@
           <t>X</t>
         </is>
       </c>
-      <c r="AD27" s="29" t="n"/>
-      <c r="AE27" s="30" t="n"/>
+      <c r="AD27" s="31" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AE27" s="32" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="31">

</xml_diff>